<commit_message>
Update completo de gráficos y tabla
</commit_message>
<xml_diff>
--- a/02_output/tables/fit_measures_models_gbmt.xlsx
+++ b/02_output/tables/fit_measures_models_gbmt.xlsx
@@ -455,13 +455,13 @@
         <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>17505.237636836</v>
+        <v>19152.134461925</v>
       </c>
       <c r="G2" t="n">
-        <v>17567.4692719864</v>
+        <v>19208.5405283422</v>
       </c>
       <c r="H2" t="n">
-        <v>-8743.61881841798</v>
+        <v>-9568.06723096248</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
@@ -496,13 +496,13 @@
         <v>15</v>
       </c>
       <c r="F3" t="n">
-        <v>74488.3928951169</v>
+        <v>41800.5568857791</v>
       </c>
       <c r="G3" t="n">
-        <v>74521.7907135327</v>
+        <v>41832.0892087501</v>
       </c>
       <c r="H3" t="n">
-        <v>-37240.1964475585</v>
+        <v>-20896.2784428895</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
@@ -537,13 +537,13 @@
         <v>16</v>
       </c>
       <c r="F4" t="n">
-        <v>1152.47955872959</v>
+        <v>1152.47955872968</v>
       </c>
       <c r="G4" t="n">
-        <v>1174.52202935996</v>
+        <v>1174.52202936005</v>
       </c>
       <c r="H4" t="n">
-        <v>-573.239779364797</v>
+        <v>-573.239779364838</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
@@ -578,13 +578,13 @@
         <v>14</v>
       </c>
       <c r="F5" t="n">
-        <v>-9231.75622899887</v>
+        <v>-10635.4451150716</v>
       </c>
       <c r="G5" t="n">
-        <v>-9176.43921997625</v>
+        <v>-10579.0390486544</v>
       </c>
       <c r="H5" t="n">
-        <v>4623.87811449943</v>
+        <v>5325.72255753579</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
@@ -619,13 +619,13 @@
         <v>15</v>
       </c>
       <c r="F6" t="n">
-        <v>-17365.6849388082</v>
+        <v>-4154.6350225228</v>
       </c>
       <c r="G6" t="n">
-        <v>-17332.2871203924</v>
+        <v>-4123.10269955176</v>
       </c>
       <c r="H6" t="n">
-        <v>8686.84246940411</v>
+        <v>2081.3175112614</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
@@ -660,13 +660,13 @@
         <v>16</v>
       </c>
       <c r="F7" t="n">
-        <v>1411.69940909925</v>
+        <v>1411.69940909922</v>
       </c>
       <c r="G7" t="n">
-        <v>1441.08936993974</v>
+        <v>1441.08936993971</v>
       </c>
       <c r="H7" t="n">
-        <v>-701.849704549623</v>
+        <v>-701.84970454961</v>
       </c>
       <c r="I7" t="n">
         <v>1</v>
@@ -701,28 +701,28 @@
         <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>8300.32404184759</v>
+        <v>8138.05928869434</v>
       </c>
       <c r="G8" t="n">
-        <v>8431.70193827631</v>
+        <v>8272.02369643522</v>
       </c>
       <c r="H8" t="n">
-        <v>-4131.1620209238</v>
+        <v>-4050.02964434717</v>
       </c>
       <c r="I8" t="n">
-        <v>0.99896216413104</v>
+        <v>0.99975885316403</v>
       </c>
       <c r="J8" t="n">
-        <v>0.000108171271523072</v>
+        <v>0.0000403174243048809</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0109369987649261</v>
+        <v>0.00240960054422001</v>
       </c>
       <c r="L8" t="n">
-        <v>976.829399235113</v>
+        <v>4256.54780064319</v>
       </c>
       <c r="M8" t="n">
-        <v>0.479166666666667</v>
+        <v>0.487272727272727</v>
       </c>
     </row>
     <row r="9">
@@ -742,28 +742,28 @@
         <v>15</v>
       </c>
       <c r="F9" t="n">
-        <v>51364.1891423727</v>
+        <v>26012.9991887665</v>
       </c>
       <c r="G9" t="n">
-        <v>51439.3342338083</v>
+        <v>26083.9469154514</v>
       </c>
       <c r="H9" t="n">
-        <v>-25673.0945711863</v>
+        <v>-12997.4995943833</v>
       </c>
       <c r="I9" t="n">
-        <v>0.998607496249679</v>
+        <v>0.998323048941198</v>
       </c>
       <c r="J9" t="n">
-        <v>0.00142695667958712</v>
+        <v>0.000771671319684808</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0161493943572312</v>
+        <v>0.0200536347585274</v>
       </c>
       <c r="L9" t="n">
-        <v>5560.61725495763</v>
+        <v>740.76461386159</v>
       </c>
       <c r="M9" t="n">
-        <v>0.45</v>
+        <v>0.438405797101449</v>
       </c>
     </row>
     <row r="10">
@@ -783,10 +783,10 @@
         <v>16</v>
       </c>
       <c r="F10" t="n">
-        <v>-5596.5359113962</v>
+        <v>-5596.53591139619</v>
       </c>
       <c r="G10" t="n">
-        <v>-5530.40849950509</v>
+        <v>-5530.40849950508</v>
       </c>
       <c r="H10" t="n">
         <v>2807.2679556981</v>
@@ -795,13 +795,13 @@
         <v>0.992061019333069</v>
       </c>
       <c r="J10" t="n">
-        <v>0.00214562387996176</v>
+        <v>0.00214562387997072</v>
       </c>
       <c r="K10" t="n">
         <v>0.0459847120555038</v>
       </c>
       <c r="L10" t="n">
-        <v>140.393195988296</v>
+        <v>140.393195988335</v>
       </c>
       <c r="M10" t="n">
         <v>0.391891891891892</v>
@@ -824,28 +824,28 @@
         <v>14</v>
       </c>
       <c r="F11" t="n">
-        <v>-21103.6319147052</v>
+        <v>-23696.0126607067</v>
       </c>
       <c r="G11" t="n">
-        <v>-20992.99789666</v>
+        <v>-23576.1497695701</v>
       </c>
       <c r="H11" t="n">
-        <v>10567.8159573526</v>
+        <v>11865.0063303533</v>
       </c>
       <c r="I11" t="n">
-        <v>0.999647156746185</v>
+        <v>0.997303087343912</v>
       </c>
       <c r="J11" t="n">
-        <v>0.000565053398012841</v>
+        <v>0.000215135532001365</v>
       </c>
       <c r="K11" t="n">
-        <v>0.00288434306663041</v>
+        <v>0.0200704633534266</v>
       </c>
       <c r="L11" t="n">
-        <v>853675719.474408</v>
+        <v>574.941572654599</v>
       </c>
       <c r="M11" t="n">
-        <v>0.191666666666667</v>
+        <v>0.203636363636364</v>
       </c>
     </row>
     <row r="12">
@@ -865,28 +865,28 @@
         <v>15</v>
       </c>
       <c r="F12" t="n">
-        <v>-58789.0669197568</v>
+        <v>-34526.4451353305</v>
       </c>
       <c r="G12" t="n">
-        <v>-58713.9218283213</v>
+        <v>-34455.4974086456</v>
       </c>
       <c r="H12" t="n">
-        <v>29403.5334598784</v>
+        <v>17272.2225676652</v>
       </c>
       <c r="I12" t="n">
-        <v>0.99973551043582</v>
+        <v>0.999972411173542</v>
       </c>
       <c r="J12" t="n">
-        <v>0.000361928361414326</v>
+        <v>0.0000129537520453665</v>
       </c>
       <c r="K12" t="n">
-        <v>0.00398880205594627</v>
+        <v>0.000171847458012433</v>
       </c>
       <c r="L12" t="n">
-        <v>40944.7551252531</v>
+        <v>332948.924345543</v>
       </c>
       <c r="M12" t="n">
-        <v>0.238636363636364</v>
+        <v>0.242753623188406</v>
       </c>
     </row>
     <row r="13">
@@ -918,7 +918,7 @@
         <v>0.999743464507726</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0000565504486137874</v>
+        <v>0.0000565504486138846</v>
       </c>
       <c r="K13" t="n">
         <v>0.00154646958950772</v>
@@ -947,28 +947,28 @@
         <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>5040.11484529363</v>
+        <v>4330.55675850808</v>
       </c>
       <c r="G14" t="n">
-        <v>5240.63900300062</v>
+        <v>4527.97799096833</v>
       </c>
       <c r="H14" t="n">
-        <v>-2491.05742264681</v>
+        <v>-2137.27837925404</v>
       </c>
       <c r="I14" t="n">
-        <v>0.99917400712242</v>
+        <v>0.998473595070283</v>
       </c>
       <c r="J14" t="n">
-        <v>0.000147612267776441</v>
+        <v>0.000317743987654754</v>
       </c>
       <c r="K14" t="n">
-        <v>0.00624277613661927</v>
+        <v>0.00977691546161557</v>
       </c>
       <c r="L14" t="n">
-        <v>2711.86094659436</v>
+        <v>1606.94028160457</v>
       </c>
       <c r="M14" t="n">
-        <v>0.241666666666667</v>
+        <v>0.258181818181818</v>
       </c>
     </row>
     <row r="15">
@@ -988,28 +988,28 @@
         <v>15</v>
       </c>
       <c r="F15" t="n">
-        <v>45821.6550474759</v>
+        <v>21053.859017124</v>
       </c>
       <c r="G15" t="n">
-        <v>45938.5474119313</v>
+        <v>21164.2221475226</v>
       </c>
       <c r="H15" t="n">
-        <v>-22896.827523738</v>
+        <v>-10512.929508562</v>
       </c>
       <c r="I15" t="n">
-        <v>0.99579103317992</v>
+        <v>0.999121042820844</v>
       </c>
       <c r="J15" t="n">
-        <v>0.00224617589824393</v>
+        <v>0.000242868198726912</v>
       </c>
       <c r="K15" t="n">
-        <v>0.0314765702337406</v>
+        <v>0.00751201142680143</v>
       </c>
       <c r="L15" t="n">
-        <v>1036.83770310261</v>
+        <v>3664.66958080104</v>
       </c>
       <c r="M15" t="n">
-        <v>0.206818181818182</v>
+        <v>0.181159420289855</v>
       </c>
     </row>
     <row r="16">
@@ -1029,25 +1029,25 @@
         <v>16</v>
       </c>
       <c r="F16" t="n">
-        <v>-9725.32969210412</v>
+        <v>-9725.3296921042</v>
       </c>
       <c r="G16" t="n">
-        <v>-9622.46482916239</v>
+        <v>-9622.46482916247</v>
       </c>
       <c r="H16" t="n">
-        <v>4876.66484605206</v>
+        <v>4876.6648460521</v>
       </c>
       <c r="I16" t="n">
         <v>0.993802729948737</v>
       </c>
       <c r="J16" t="n">
-        <v>0.00123996740879262</v>
+        <v>0.00123996740879151</v>
       </c>
       <c r="K16" t="n">
         <v>0.0388139087052969</v>
       </c>
       <c r="L16" t="n">
-        <v>434.499122593514</v>
+        <v>434.499122593479</v>
       </c>
       <c r="M16" t="n">
         <v>0.259459459459459</v>
@@ -1070,28 +1070,28 @@
         <v>14</v>
       </c>
       <c r="F17" t="n">
-        <v>-22559.0260670695</v>
+        <v>-32176.6414672006</v>
       </c>
       <c r="G17" t="n">
-        <v>-22365.4165354904</v>
+        <v>-31986.2709930425</v>
       </c>
       <c r="H17" t="n">
-        <v>11307.5130335348</v>
+        <v>16115.3207336003</v>
       </c>
       <c r="I17" t="n">
-        <v>0.999446242221777</v>
+        <v>0.999541413955656</v>
       </c>
       <c r="J17" t="n">
-        <v>0.0000542996043433388</v>
+        <v>0.000308376960366887</v>
       </c>
       <c r="K17" t="n">
-        <v>0.00466068906560473</v>
+        <v>0.00353087113274833</v>
       </c>
       <c r="L17" t="n">
-        <v>1394.26085129017</v>
+        <v>2610651893.58003</v>
       </c>
       <c r="M17" t="n">
-        <v>0.00833333333333333</v>
+        <v>0.170909090909091</v>
       </c>
     </row>
     <row r="18">
@@ -1111,28 +1111,28 @@
         <v>15</v>
       </c>
       <c r="F18" t="n">
-        <v>-76120.0353604905</v>
+        <v>-40149.8887672495</v>
       </c>
       <c r="G18" t="n">
-        <v>-76003.1429960351</v>
+        <v>-40039.5256368509</v>
       </c>
       <c r="H18" t="n">
-        <v>38074.0176802452</v>
+        <v>20088.9443836248</v>
       </c>
       <c r="I18" t="n">
-        <v>0.99992564317642</v>
+        <v>0.999204147229496</v>
       </c>
       <c r="J18" t="n">
-        <v>0.00000975956249313348</v>
+        <v>0.00105457516972648</v>
       </c>
       <c r="K18" t="n">
-        <v>0.000621409751813596</v>
+        <v>0.0073537247618258</v>
       </c>
       <c r="L18" t="n">
-        <v>109923.485107077</v>
+        <v>40022.5324651492</v>
       </c>
       <c r="M18" t="n">
-        <v>0.195454545454545</v>
+        <v>0.0579710144927536</v>
       </c>
     </row>
     <row r="19">
@@ -1158,19 +1158,19 @@
         <v>-24801.398752701</v>
       </c>
       <c r="H19" t="n">
-        <v>12466.1318078213</v>
+        <v>12466.1318078214</v>
       </c>
       <c r="I19" t="n">
-        <v>0.997107423908402</v>
+        <v>0.997107423908403</v>
       </c>
       <c r="J19" t="n">
-        <v>0.000545493509648008</v>
+        <v>0.000545493509649173</v>
       </c>
       <c r="K19" t="n">
         <v>0.0269737842364459</v>
       </c>
       <c r="L19" t="n">
-        <v>1130.36616102886</v>
+        <v>1130.36616103104</v>
       </c>
       <c r="M19" t="n">
         <v>0.175675675675676</v>
@@ -1193,28 +1193,28 @@
         <v>14</v>
       </c>
       <c r="F20" t="n">
-        <v>5910.57953693224</v>
+        <v>3289.0029090206</v>
       </c>
       <c r="G20" t="n">
-        <v>6180.2499559175</v>
+        <v>3556.93172450237</v>
       </c>
       <c r="H20" t="n">
-        <v>-2916.28976846612</v>
+        <v>-1606.5014545103</v>
       </c>
       <c r="I20" t="n">
-        <v>0.995301748095798</v>
+        <v>0.997865701337383</v>
       </c>
       <c r="J20" t="n">
-        <v>0.000929947402544935</v>
+        <v>0.000139326711671451</v>
       </c>
       <c r="K20" t="n">
-        <v>0.024191439954068</v>
+        <v>0.015185387307663</v>
       </c>
       <c r="L20" t="n">
-        <v>318517.416093053</v>
+        <v>48138.6252620519</v>
       </c>
       <c r="M20" t="n">
-        <v>0.0666666666666667</v>
+        <v>0.0545454545454545</v>
       </c>
     </row>
     <row r="21">
@@ -1234,28 +1234,28 @@
         <v>15</v>
       </c>
       <c r="F21" t="n">
-        <v>37776.5340582798</v>
+        <v>17881.0779196504</v>
       </c>
       <c r="G21" t="n">
-        <v>37935.1736957549</v>
+        <v>18030.8564537628</v>
       </c>
       <c r="H21" t="n">
-        <v>-18869.2670291399</v>
+        <v>-8921.53895982521</v>
       </c>
       <c r="I21" t="n">
-        <v>0.99705310505623</v>
+        <v>0.996613048711138</v>
       </c>
       <c r="J21" t="n">
-        <v>0.000296896074025985</v>
+        <v>0.000701503144901708</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0226225544841956</v>
+        <v>0.0212851668091425</v>
       </c>
       <c r="L21" t="n">
-        <v>4434.71735126719</v>
+        <v>4607.25237187668</v>
       </c>
       <c r="M21" t="n">
-        <v>0.211363636363636</v>
+        <v>0.181159420289855</v>
       </c>
     </row>
     <row r="22">
@@ -1284,16 +1284,16 @@
         <v>5587.25939087767</v>
       </c>
       <c r="I22" t="n">
-        <v>0.990639256458825</v>
+        <v>0.990639256458824</v>
       </c>
       <c r="J22" t="n">
-        <v>0.000386452145444929</v>
+        <v>0.000386452145446414</v>
       </c>
       <c r="K22" t="n">
         <v>0.0426036394641168</v>
       </c>
       <c r="L22" t="n">
-        <v>361.4783191744</v>
+        <v>361.478319174255</v>
       </c>
       <c r="M22" t="n">
         <v>0.183783783783784</v>
@@ -1316,28 +1316,28 @@
         <v>14</v>
       </c>
       <c r="F23" t="n">
-        <v>-30294.9533010103</v>
+        <v>-34958.768888461</v>
       </c>
       <c r="G23" t="n">
-        <v>-30046.0267604085</v>
+        <v>-34697.8908312814</v>
       </c>
       <c r="H23" t="n">
-        <v>15183.4766505051</v>
+        <v>17516.3844442305</v>
       </c>
       <c r="I23" t="n">
-        <v>0.999526017851371</v>
+        <v>0.998769868382734</v>
       </c>
       <c r="J23" t="n">
-        <v>0.00016996892106555</v>
+        <v>0.000581366046689112</v>
       </c>
       <c r="K23" t="n">
-        <v>0.00323503149143924</v>
+        <v>0.00818022696338202</v>
       </c>
       <c r="L23" t="n">
-        <v>76416490.581779</v>
+        <v>5440971.66135695</v>
       </c>
       <c r="M23" t="n">
-        <v>0.00833333333333333</v>
+        <v>0.0509090909090909</v>
       </c>
     </row>
     <row r="24">
@@ -1357,28 +1357,28 @@
         <v>15</v>
       </c>
       <c r="F24" t="n">
-        <v>-83178.8106487214</v>
+        <v>-47505.8621681971</v>
       </c>
       <c r="G24" t="n">
-        <v>-83020.1710112463</v>
+        <v>-47356.0836340847</v>
       </c>
       <c r="H24" t="n">
-        <v>41608.4053243607</v>
+        <v>23771.9310840986</v>
       </c>
       <c r="I24" t="n">
-        <v>0.998306416701757</v>
+        <v>0.999589394560058</v>
       </c>
       <c r="J24" t="n">
-        <v>0.000599619746200378</v>
+        <v>0.000171800514453953</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0132809147305643</v>
+        <v>0.00245721378520987</v>
       </c>
       <c r="L24" t="n">
-        <v>315788406.59252</v>
+        <v>420091.171902427</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0727272727272727</v>
+        <v>0.0579710144927536</v>
       </c>
     </row>
     <row r="25">
@@ -1410,13 +1410,13 @@
         <v>0.996971368261262</v>
       </c>
       <c r="J25" t="n">
-        <v>0.00113112720084189</v>
+        <v>0.00113112720084247</v>
       </c>
       <c r="K25" t="n">
         <v>0.0180459662763897</v>
       </c>
       <c r="L25" t="n">
-        <v>7395.24512878382</v>
+        <v>7395.24512878858</v>
       </c>
       <c r="M25" t="n">
         <v>0.0972972972972973</v>
@@ -1439,28 +1439,28 @@
         <v>14</v>
       </c>
       <c r="F26" t="n">
-        <v>2394.87160092105</v>
+        <v>741.771060571764</v>
       </c>
       <c r="G26" t="n">
-        <v>2726.77365505675</v>
+        <v>1080.20745907505</v>
       </c>
       <c r="H26" t="n">
-        <v>-1149.43580046052</v>
+        <v>-322.885530285882</v>
       </c>
       <c r="I26" t="n">
-        <v>0.998370032400607</v>
+        <v>0.99664241880978</v>
       </c>
       <c r="J26" t="n">
-        <v>0.000227237415675556</v>
+        <v>0.000350888873395637</v>
       </c>
       <c r="K26" t="n">
-        <v>0.0106863599381461</v>
+        <v>0.0171449549098299</v>
       </c>
       <c r="L26" t="n">
-        <v>954651.376268639</v>
+        <v>2349.46971854796</v>
       </c>
       <c r="M26" t="n">
-        <v>0.0583333333333333</v>
+        <v>0.0618181818181818</v>
       </c>
     </row>
     <row r="27">
@@ -1480,28 +1480,28 @@
         <v>15</v>
       </c>
       <c r="F27" t="n">
-        <v>35743.5692195552</v>
+        <v>16839.6144806652</v>
       </c>
       <c r="G27" t="n">
-        <v>35943.9561300501</v>
+        <v>17028.8084184914</v>
       </c>
       <c r="H27" t="n">
-        <v>-17847.7846097776</v>
+        <v>-8395.8072403326</v>
       </c>
       <c r="I27" t="n">
-        <v>0.997862657486091</v>
+        <v>0.997053710214473</v>
       </c>
       <c r="J27" t="n">
-        <v>0.000498142627817941</v>
+        <v>0.000520623058851045</v>
       </c>
       <c r="K27" t="n">
-        <v>0.0125389491741425</v>
+        <v>0.0165681430116176</v>
       </c>
       <c r="L27" t="n">
-        <v>2421.82219132139</v>
+        <v>41088.5403295119</v>
       </c>
       <c r="M27" t="n">
-        <v>0.118181818181818</v>
+        <v>0.0543478260869565</v>
       </c>
     </row>
     <row r="28">
@@ -1527,19 +1527,19 @@
         <v>-12034.1739213946</v>
       </c>
       <c r="H28" t="n">
-        <v>6129.25684321879</v>
+        <v>6129.2568432188</v>
       </c>
       <c r="I28" t="n">
         <v>0.988618451214155</v>
       </c>
       <c r="J28" t="n">
-        <v>0.00118864511138501</v>
+        <v>0.00118864511138415</v>
       </c>
       <c r="K28" t="n">
         <v>0.0436290429116754</v>
       </c>
       <c r="L28" t="n">
-        <v>503.437357825941</v>
+        <v>503.437357825711</v>
       </c>
       <c r="M28" t="n">
         <v>0.102702702702703</v>
@@ -1562,28 +1562,28 @@
         <v>14</v>
       </c>
       <c r="F29" t="n">
-        <v>-33520.6827173972</v>
+        <v>-38583.4528414676</v>
       </c>
       <c r="G29" t="n">
-        <v>-33195.6952893893</v>
+        <v>-38237.9656846622</v>
       </c>
       <c r="H29" t="n">
-        <v>16807.3413586986</v>
+        <v>19340.7264207338</v>
       </c>
       <c r="I29" t="n">
-        <v>0.998153164636392</v>
+        <v>0.999253272427098</v>
       </c>
       <c r="J29" t="n">
-        <v>0.000613160101187318</v>
+        <v>0.000179142029742041</v>
       </c>
       <c r="K29" t="n">
-        <v>0.0120358325170879</v>
+        <v>0.0040351742832434</v>
       </c>
       <c r="L29" t="n">
-        <v>1076310.89518605</v>
+        <v>183078.128701686</v>
       </c>
       <c r="M29" t="n">
-        <v>0.00833333333333333</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="30">
@@ -1603,28 +1603,28 @@
         <v>15</v>
       </c>
       <c r="F30" t="n">
-        <v>-87511.5305501154</v>
+        <v>-50755.1322565055</v>
       </c>
       <c r="G30" t="n">
-        <v>-87311.1436396205</v>
+        <v>-50565.9383186793</v>
       </c>
       <c r="H30" t="n">
-        <v>43779.7652750577</v>
+        <v>25401.5661282528</v>
       </c>
       <c r="I30" t="n">
-        <v>0.998091768270823</v>
+        <v>0.998276294115325</v>
       </c>
       <c r="J30" t="n">
-        <v>0.000444060772361868</v>
+        <v>0.000375908203855026</v>
       </c>
       <c r="K30" t="n">
-        <v>0.0108143268798827</v>
+        <v>0.00998778881448423</v>
       </c>
       <c r="L30" t="n">
-        <v>15243.4815709417</v>
+        <v>218118.227469422</v>
       </c>
       <c r="M30" t="n">
-        <v>0.0363636363636364</v>
+        <v>0.0543478260869565</v>
       </c>
     </row>
     <row r="31">
@@ -1653,10 +1653,10 @@
         <v>14354.9802814135</v>
       </c>
       <c r="I31" t="n">
-        <v>0.995756994115181</v>
+        <v>0.995756994115182</v>
       </c>
       <c r="J31" t="n">
-        <v>0.000636178713437852</v>
+        <v>0.000636178713437543</v>
       </c>
       <c r="K31" t="n">
         <v>0.0213084593128611</v>
@@ -1685,28 +1685,28 @@
         <v>14</v>
       </c>
       <c r="F32" t="n">
-        <v>222.454519875809</v>
+        <v>29.5524637562906</v>
       </c>
       <c r="G32" t="n">
-        <v>630.41746141761</v>
+        <v>445.547203583242</v>
       </c>
       <c r="H32" t="n">
-        <v>-52.2272599379043</v>
+        <v>44.2237681218547</v>
       </c>
       <c r="I32" t="n">
-        <v>0.998843273788869</v>
+        <v>0.997460259448039</v>
       </c>
       <c r="J32" t="n">
-        <v>0.000336506756031349</v>
+        <v>0.000386768956558808</v>
       </c>
       <c r="K32" t="n">
-        <v>0.00713148312664425</v>
+        <v>0.0138010306504396</v>
       </c>
       <c r="L32" t="n">
-        <v>209362.239774149</v>
+        <v>4933625759001.09</v>
       </c>
       <c r="M32" t="n">
-        <v>0.0291666666666667</v>
+        <v>0.0218181818181818</v>
       </c>
     </row>
     <row r="33">
@@ -1726,28 +1726,28 @@
         <v>15</v>
       </c>
       <c r="F33" t="n">
-        <v>32534.9878450433</v>
+        <v>14389.2012532173</v>
       </c>
       <c r="G33" t="n">
-        <v>32777.1220285579</v>
+        <v>14617.8105947573</v>
       </c>
       <c r="H33" t="n">
-        <v>-16238.4939225216</v>
+        <v>-7165.60062660865</v>
       </c>
       <c r="I33" t="n">
-        <v>0.997957909530393</v>
+        <v>0.996254714872452</v>
       </c>
       <c r="J33" t="n">
-        <v>0.00038507116864214</v>
+        <v>0.000634743400761863</v>
       </c>
       <c r="K33" t="n">
-        <v>0.0108452706801463</v>
+        <v>0.0194012837881666</v>
       </c>
       <c r="L33" t="n">
-        <v>3508.91977774726</v>
+        <v>4722.3229890392</v>
       </c>
       <c r="M33" t="n">
-        <v>0.104545454545455</v>
+        <v>0.0543478260869565</v>
       </c>
     </row>
     <row r="34">
@@ -1767,28 +1767,28 @@
         <v>14</v>
       </c>
       <c r="F34" t="n">
-        <v>-35251.6511798205</v>
+        <v>-41561.7244983378</v>
       </c>
       <c r="G34" t="n">
-        <v>-34857.5174905344</v>
+        <v>-41152.780516813</v>
       </c>
       <c r="H34" t="n">
-        <v>17682.8255899103</v>
+        <v>20838.8622491689</v>
       </c>
       <c r="I34" t="n">
-        <v>0.999548831870017</v>
+        <v>0.998954386016592</v>
       </c>
       <c r="J34" t="n">
-        <v>0.000258427437583574</v>
+        <v>0.000250375264365856</v>
       </c>
       <c r="K34" t="n">
-        <v>0.0034817534393506</v>
+        <v>0.00649797440832078</v>
       </c>
       <c r="L34" t="n">
-        <v>19791501409.2408</v>
+        <v>99825807.2208076</v>
       </c>
       <c r="M34" t="n">
-        <v>0.00833333333333333</v>
+        <v>0.0509090909090909</v>
       </c>
     </row>
     <row r="35">
@@ -1808,28 +1808,28 @@
         <v>15</v>
       </c>
       <c r="F35" t="n">
-        <v>-92423.8555528099</v>
+        <v>-52560.5593551516</v>
       </c>
       <c r="G35" t="n">
-        <v>-92181.7213692952</v>
+        <v>-52331.9500136116</v>
       </c>
       <c r="H35" t="n">
-        <v>46240.9277764049</v>
+        <v>26309.2796775758</v>
       </c>
       <c r="I35" t="n">
-        <v>0.998742285411797</v>
+        <v>0.999460008508341</v>
       </c>
       <c r="J35" t="n">
-        <v>0.000175298994313748</v>
+        <v>0.0000925544501731064</v>
       </c>
       <c r="K35" t="n">
-        <v>0.00792069642514007</v>
+        <v>0.00264754430633474</v>
       </c>
       <c r="L35" t="n">
-        <v>37865.4533549</v>
+        <v>18430944450.762</v>
       </c>
       <c r="M35" t="n">
-        <v>0.0363636363636364</v>
+        <v>0.0398550724637681</v>
       </c>
     </row>
     <row r="36">
@@ -1852,22 +1852,22 @@
         <v>-31802.493130674</v>
       </c>
       <c r="G36" t="n">
-        <v>-31589.4159145804</v>
+        <v>-31589.4159145805</v>
       </c>
       <c r="H36" t="n">
         <v>15930.246565337</v>
       </c>
       <c r="I36" t="n">
-        <v>0.994209157004286</v>
+        <v>0.994209157004285</v>
       </c>
       <c r="J36" t="n">
-        <v>0.000571522718577174</v>
+        <v>0.000571522718577673</v>
       </c>
       <c r="K36" t="n">
         <v>0.0250763316538558</v>
       </c>
       <c r="L36" t="n">
-        <v>6329.006659703</v>
+        <v>6329.00665970273</v>
       </c>
       <c r="M36" t="n">
         <v>0.0405405405405405</v>
@@ -1890,28 +1890,28 @@
         <v>14</v>
       </c>
       <c r="F37" t="n">
-        <v>-1280.77918869832</v>
+        <v>-1738.96967327442</v>
       </c>
       <c r="G37" t="n">
-        <v>-810.584612006073</v>
+        <v>-1252.46735042595</v>
       </c>
       <c r="H37" t="n">
-        <v>708.389594349159</v>
+        <v>938.484836637212</v>
       </c>
       <c r="I37" t="n">
-        <v>0.99834785892196</v>
+        <v>0.998415369714549</v>
       </c>
       <c r="J37" t="n">
-        <v>0.00022756474707912</v>
+        <v>0.000560442716415779</v>
       </c>
       <c r="K37" t="n">
-        <v>0.00908107027999574</v>
+        <v>0.00845616728778432</v>
       </c>
       <c r="L37" t="n">
-        <v>10168055.0859311</v>
+        <v>166731122589824</v>
       </c>
       <c r="M37" t="n">
-        <v>0.0291666666666667</v>
+        <v>0.0218181818181818</v>
       </c>
     </row>
     <row r="38">
@@ -1931,28 +1931,28 @@
         <v>15</v>
       </c>
       <c r="F38" t="n">
-        <v>31956.1064529683</v>
+        <v>13184.741553377</v>
       </c>
       <c r="G38" t="n">
-        <v>32239.9879095028</v>
+        <v>13452.7662986308</v>
       </c>
       <c r="H38" t="n">
-        <v>-15944.0532264842</v>
+        <v>-6558.3707766885</v>
       </c>
       <c r="I38" t="n">
-        <v>0.994959466326592</v>
+        <v>0.99681557211954</v>
       </c>
       <c r="J38" t="n">
-        <v>0.000536460833620075</v>
+        <v>0.000489136364462202</v>
       </c>
       <c r="K38" t="n">
-        <v>0.0261728417426142</v>
+        <v>0.0176644229111068</v>
       </c>
       <c r="L38" t="n">
-        <v>5511.89662039159</v>
+        <v>15638.5232908415</v>
       </c>
       <c r="M38" t="n">
-        <v>0.0386363636363636</v>
+        <v>0.0543478260869565</v>
       </c>
     </row>
     <row r="39">
@@ -1972,28 +1972,28 @@
         <v>14</v>
       </c>
       <c r="F39" t="n">
-        <v>-36928.0396260399</v>
+        <v>-42907.0286265868</v>
       </c>
       <c r="G39" t="n">
-        <v>-36457.8450493476</v>
+        <v>-42420.5263037383</v>
       </c>
       <c r="H39" t="n">
-        <v>18532.0198130199</v>
+        <v>21522.5143132934</v>
       </c>
       <c r="I39" t="n">
-        <v>0.999424228176969</v>
+        <v>0.998987974653571</v>
       </c>
       <c r="J39" t="n">
-        <v>0.00015661804243078</v>
+        <v>0.000277250343724179</v>
       </c>
       <c r="K39" t="n">
-        <v>0.00299525725295936</v>
+        <v>0.00450373868872747</v>
       </c>
       <c r="L39" t="n">
-        <v>21315567048.8742</v>
+        <v>392806415.69629</v>
       </c>
       <c r="M39" t="n">
-        <v>0.00833333333333333</v>
+        <v>0.0218181818181818</v>
       </c>
     </row>
     <row r="40">
@@ -2013,28 +2013,28 @@
         <v>15</v>
       </c>
       <c r="F40" t="n">
-        <v>-94725.1270400058</v>
+        <v>-54182.6315737896</v>
       </c>
       <c r="G40" t="n">
-        <v>-94441.2455834713</v>
+        <v>-53914.6068285359</v>
       </c>
       <c r="H40" t="n">
-        <v>47396.5635200029</v>
+        <v>27125.3157868948</v>
       </c>
       <c r="I40" t="n">
-        <v>0.999305957211512</v>
+        <v>0.999202842312359</v>
       </c>
       <c r="J40" t="n">
-        <v>0.00015879419578236</v>
+        <v>0.000139936000525408</v>
       </c>
       <c r="K40" t="n">
-        <v>0.00409725591003832</v>
+        <v>0.0047030342464313</v>
       </c>
       <c r="L40" t="n">
-        <v>196564540.611979</v>
+        <v>670312646.962996</v>
       </c>
       <c r="M40" t="n">
-        <v>0.0318181818181818</v>
+        <v>0.0398550724637681</v>
       </c>
     </row>
     <row r="41">
@@ -2063,10 +2063,10 @@
         <v>16019.9166516636</v>
       </c>
       <c r="I41" t="n">
-        <v>0.996497496902979</v>
+        <v>0.996497496902982</v>
       </c>
       <c r="J41" t="n">
-        <v>0.000490252338873427</v>
+        <v>0.000490252338872123</v>
       </c>
       <c r="K41" t="n">
         <v>0.0199604409240764</v>
@@ -2095,28 +2095,28 @@
         <v>14</v>
       </c>
       <c r="F42" t="n">
-        <v>-2527.03681683356</v>
+        <v>-3238.53426862406</v>
       </c>
       <c r="G42" t="n">
-        <v>-1980.78135273522</v>
+        <v>-2681.52436275407</v>
       </c>
       <c r="H42" t="n">
-        <v>1342.51840841678</v>
+        <v>1698.26713431203</v>
       </c>
       <c r="I42" t="n">
-        <v>0.998393210033437</v>
+        <v>0.998552841121495</v>
       </c>
       <c r="J42" t="n">
-        <v>0.000228089553151282</v>
+        <v>0.000351169044476902</v>
       </c>
       <c r="K42" t="n">
-        <v>0.00705877647801817</v>
+        <v>0.00793915843603546</v>
       </c>
       <c r="L42" t="n">
-        <v>20536491.3376515</v>
+        <v>13918602.9725197</v>
       </c>
       <c r="M42" t="n">
-        <v>0.0291666666666667</v>
+        <v>0.0254545454545455</v>
       </c>
     </row>
     <row r="43">
@@ -2136,28 +2136,28 @@
         <v>15</v>
       </c>
       <c r="F43" t="n">
-        <v>30156.8781094165</v>
+        <v>12791.8680047178</v>
       </c>
       <c r="G43" t="n">
-        <v>30474.1573843667</v>
+        <v>13099.3081536854</v>
       </c>
       <c r="H43" t="n">
-        <v>-15040.4390547082</v>
+        <v>-6356.93400235891</v>
       </c>
       <c r="I43" t="n">
-        <v>0.996797319144393</v>
+        <v>0.999373893127903</v>
       </c>
       <c r="J43" t="n">
-        <v>0.000448704400659194</v>
+        <v>0.000124554989555947</v>
       </c>
       <c r="K43" t="n">
-        <v>0.0172584669885934</v>
+        <v>0.0034509334746487</v>
       </c>
       <c r="L43" t="n">
-        <v>5659.30447293227</v>
+        <v>4699781133.20584</v>
       </c>
       <c r="M43" t="n">
-        <v>0.0272727272727273</v>
+        <v>0.0181159420289855</v>
       </c>
     </row>
     <row r="44">
@@ -2177,28 +2177,26 @@
         <v>14</v>
       </c>
       <c r="F44" t="n">
-        <v>-38428.725129709</v>
+        <v>-43452.1519781235</v>
       </c>
       <c r="G44" t="n">
-        <v>-37896.2989178663</v>
+        <v>-42902.1928305556</v>
       </c>
       <c r="H44" t="n">
-        <v>19291.3625648545</v>
+        <v>21804.0759890617</v>
       </c>
       <c r="I44" t="n">
-        <v>0.998529444655771</v>
+        <v>0.999278607875967</v>
       </c>
       <c r="J44" t="n">
-        <v>0.000323024071161755</v>
-      </c>
-      <c r="K44" t="n">
-        <v>0.00587642503914021</v>
-      </c>
+        <v>0.000190089757306094</v>
+      </c>
+      <c r="K44"/>
       <c r="L44" t="n">
-        <v>7601826.6578025</v>
+        <v>14466030.8470494</v>
       </c>
       <c r="M44" t="n">
-        <v>0.00833333333333333</v>
+        <v>0.00363636363636364</v>
       </c>
     </row>
     <row r="45">
@@ -2218,28 +2216,28 @@
         <v>15</v>
       </c>
       <c r="F45" t="n">
-        <v>-96342.5123205172</v>
+        <v>-55688.3139202797</v>
       </c>
       <c r="G45" t="n">
-        <v>-96016.8835909631</v>
+        <v>-55380.8737713121</v>
       </c>
       <c r="H45" t="n">
-        <v>48210.2561602586</v>
+        <v>27883.1569601398</v>
       </c>
       <c r="I45" t="n">
-        <v>0.998306664305605</v>
+        <v>0.999508386570424</v>
       </c>
       <c r="J45" t="n">
-        <v>0.000190556194991027</v>
+        <v>0.000113590683364489</v>
       </c>
       <c r="K45" t="n">
-        <v>0.010755038864769</v>
+        <v>0.00329533571269318</v>
       </c>
       <c r="L45" t="n">
-        <v>31447.1031707953</v>
+        <v>6747930.73979365</v>
       </c>
       <c r="M45" t="n">
-        <v>0.0227272727272727</v>
+        <v>0.0144927536231884</v>
       </c>
     </row>
     <row r="46">
@@ -2268,10 +2266,10 @@
         <v>16710.9527041926</v>
       </c>
       <c r="I46" t="n">
-        <v>0.996334542522386</v>
+        <v>0.996334542522385</v>
       </c>
       <c r="J46" t="n">
-        <v>0.000374998471986249</v>
+        <v>0.000374998471987012</v>
       </c>
       <c r="K46"/>
       <c r="L46" t="n">
@@ -2298,28 +2296,28 @@
         <v>14</v>
       </c>
       <c r="F47" t="n">
-        <v>-2770.18977845865</v>
+        <v>-3637.33995228324</v>
       </c>
       <c r="G47" t="n">
-        <v>-2161.70267920986</v>
+        <v>-3009.82246339173</v>
       </c>
       <c r="H47" t="n">
-        <v>1473.09488922932</v>
+        <v>1907.66997614162</v>
       </c>
       <c r="I47" t="n">
-        <v>0.999766515288041</v>
+        <v>0.99657139853151</v>
       </c>
       <c r="J47" t="n">
-        <v>0.0000491178490182544</v>
+        <v>0.000427347778500162</v>
       </c>
       <c r="K47" t="n">
-        <v>0.000942565511876546</v>
+        <v>0.0155992785200554</v>
       </c>
       <c r="L47" t="n">
-        <v>10236835.1882615</v>
+        <v>9570062.08067453</v>
       </c>
       <c r="M47" t="n">
-        <v>0.025</v>
+        <v>0.0254545454545455</v>
       </c>
     </row>
     <row r="48">
@@ -2339,28 +2337,28 @@
         <v>15</v>
       </c>
       <c r="F48" t="n">
-        <v>29174.6554984901</v>
+        <v>12417.7320114333</v>
       </c>
       <c r="G48" t="n">
-        <v>29533.6820464601</v>
+        <v>12764.5875641147</v>
       </c>
       <c r="H48" t="n">
-        <v>-14544.327749245</v>
+        <v>-6164.86600571666</v>
       </c>
       <c r="I48" t="n">
-        <v>0.997115910738381</v>
+        <v>0.999028514770846</v>
       </c>
       <c r="J48" t="n">
-        <v>0.000147917347148749</v>
+        <v>0.00022857966092579</v>
       </c>
       <c r="K48" t="n">
-        <v>0.0129499529100454</v>
+        <v>0.00583218315477055</v>
       </c>
       <c r="L48" t="n">
-        <v>5209.76413964709</v>
+        <v>13560838907616746</v>
       </c>
       <c r="M48" t="n">
-        <v>0.0272727272727273</v>
+        <v>0.0108695652173913</v>
       </c>
     </row>
     <row r="49">
@@ -2380,28 +2378,26 @@
         <v>14</v>
       </c>
       <c r="F49" t="n">
-        <v>-39617.7967109101</v>
+        <v>-43705.5081403673</v>
       </c>
       <c r="G49" t="n">
-        <v>-39009.3096116613</v>
+        <v>-43085.0414097779</v>
       </c>
       <c r="H49" t="n">
-        <v>19896.898355455</v>
+        <v>21940.7540701836</v>
       </c>
       <c r="I49" t="n">
-        <v>0.997495135411269</v>
+        <v>0.999358762556415</v>
       </c>
       <c r="J49" t="n">
-        <v>0.000281845975318024</v>
-      </c>
-      <c r="K49" t="n">
-        <v>0.0138542744744293</v>
-      </c>
+        <v>0.000168968673160972</v>
+      </c>
+      <c r="K49"/>
       <c r="L49" t="n">
-        <v>6516141.05281544</v>
+        <v>12858805.0862661</v>
       </c>
       <c r="M49" t="n">
-        <v>0.00833333333333333</v>
+        <v>0.00363636363636364</v>
       </c>
     </row>
     <row r="50">
@@ -2421,28 +2417,28 @@
         <v>15</v>
       </c>
       <c r="F50" t="n">
-        <v>-96795.6867734645</v>
+        <v>-56210.9147559452</v>
       </c>
       <c r="G50" t="n">
-        <v>-96428.3107708905</v>
+        <v>-55864.0592032639</v>
       </c>
       <c r="H50" t="n">
-        <v>48441.8433867323</v>
+        <v>28149.4573779726</v>
       </c>
       <c r="I50" t="n">
-        <v>0.998489806951499</v>
+        <v>0.999341951307762</v>
       </c>
       <c r="J50" t="n">
-        <v>0.000170093827569558</v>
+        <v>0.0000635607687984982</v>
       </c>
       <c r="K50" t="n">
-        <v>0.00959212369376056</v>
+        <v>0.00273052859122958</v>
       </c>
       <c r="L50" t="n">
-        <v>861750.702484412</v>
+        <v>18771925.1092428</v>
       </c>
       <c r="M50" t="n">
-        <v>0.00909090909090909</v>
+        <v>0.0144927536231884</v>
       </c>
     </row>
     <row r="51">
@@ -2462,7 +2458,7 @@
         <v>16</v>
       </c>
       <c r="F51" t="n">
-        <v>-32799.5049261363</v>
+        <v>-32799.5049261362</v>
       </c>
       <c r="G51" t="n">
         <v>-32476.2153568908</v>
@@ -2471,10 +2467,10 @@
         <v>16443.7524630681</v>
       </c>
       <c r="I51" t="n">
-        <v>0.994915470109983</v>
+        <v>0.994915470109981</v>
       </c>
       <c r="J51" t="n">
-        <v>0.000404601392544504</v>
+        <v>0.000404601392545363</v>
       </c>
       <c r="K51"/>
       <c r="L51" t="n">
@@ -2501,28 +2497,28 @@
         <v>14</v>
       </c>
       <c r="F52" t="n">
-        <v>-3253.13510269248</v>
+        <v>-4430.08249520362</v>
       </c>
       <c r="G52" t="n">
-        <v>-2568.58711603759</v>
+        <v>-3739.10818159275</v>
       </c>
       <c r="H52" t="n">
-        <v>1725.56755134624</v>
+        <v>2313.04124760181</v>
       </c>
       <c r="I52" t="n">
-        <v>0.99900675638604</v>
+        <v>0.997145680644905</v>
       </c>
       <c r="J52" t="n">
-        <v>0.000188277437325233</v>
+        <v>0.0003415136534406</v>
       </c>
       <c r="K52" t="n">
-        <v>0.00414024086387938</v>
+        <v>0.011445375458655</v>
       </c>
       <c r="L52" t="n">
-        <v>638587776.691683</v>
+        <v>5048061.36907921</v>
       </c>
       <c r="M52" t="n">
-        <v>0.0208333333333333</v>
+        <v>0.0181818181818182</v>
       </c>
     </row>
     <row r="53">
@@ -2542,28 +2538,28 @@
         <v>15</v>
       </c>
       <c r="F53" t="n">
-        <v>28494.2411244043</v>
+        <v>11990.1273852637</v>
       </c>
       <c r="G53" t="n">
-        <v>28903.364399998</v>
+        <v>12376.3983416589</v>
       </c>
       <c r="H53" t="n">
-        <v>-14198.1205622022</v>
+        <v>-5946.06369263186</v>
       </c>
       <c r="I53" t="n">
-        <v>0.995603813937169</v>
+        <v>0.997930513441405</v>
       </c>
       <c r="J53" t="n">
-        <v>0.000759037530298666</v>
+        <v>0.000442856981189741</v>
       </c>
       <c r="K53" t="n">
-        <v>0.0201534411977775</v>
+        <v>0.00883827882513091</v>
       </c>
       <c r="L53" t="n">
-        <v>34449634.7195528</v>
+        <v>121440373884137</v>
       </c>
       <c r="M53" t="n">
-        <v>0.025</v>
+        <v>0.0108695652173913</v>
       </c>
     </row>
     <row r="54">
@@ -2583,28 +2579,26 @@
         <v>14</v>
       </c>
       <c r="F54" t="n">
-        <v>-40966.477311135</v>
+        <v>-45143.1526877801</v>
       </c>
       <c r="G54" t="n">
-        <v>-40309.5878289914</v>
+        <v>-44452.1783741693</v>
       </c>
       <c r="H54" t="n">
-        <v>20578.2386555675</v>
+        <v>22669.5763438901</v>
       </c>
       <c r="I54" t="n">
-        <v>0.999654482612349</v>
+        <v>0.998693326466874</v>
       </c>
       <c r="J54" t="n">
-        <v>0.0000707201936256188</v>
-      </c>
-      <c r="K54" t="n">
-        <v>0.00157238792001957</v>
-      </c>
+        <v>0.000195303768907372</v>
+      </c>
+      <c r="K54"/>
       <c r="L54" t="n">
-        <v>4039227714.63468</v>
+        <v>6737434229.34035</v>
       </c>
       <c r="M54" t="n">
-        <v>0.00833333333333333</v>
+        <v>0.00363636363636364</v>
       </c>
     </row>
     <row r="55">
@@ -2624,28 +2618,26 @@
         <v>15</v>
       </c>
       <c r="F55" t="n">
-        <v>-97917.9556237421</v>
+        <v>-58391.3367204267</v>
       </c>
       <c r="G55" t="n">
-        <v>-97508.8323481484</v>
+        <v>-58005.0657640315</v>
       </c>
       <c r="H55" t="n">
-        <v>49007.9778118711</v>
+        <v>29244.6683602133</v>
       </c>
       <c r="I55" t="n">
-        <v>0.998818272891435</v>
+        <v>0.998796142737754</v>
       </c>
       <c r="J55" t="n">
-        <v>0.00019483575014047</v>
-      </c>
-      <c r="K55" t="n">
-        <v>0.00571503431705423</v>
-      </c>
+        <v>0.000430306811590074</v>
+      </c>
+      <c r="K55"/>
       <c r="L55" t="n">
-        <v>770367.516406361</v>
+        <v>649892.521291533</v>
       </c>
       <c r="M55" t="n">
-        <v>0.00909090909090909</v>
+        <v>0.0036231884057971</v>
       </c>
     </row>
     <row r="56">
@@ -2677,7 +2669,7 @@
         <v>0.996139684289096</v>
       </c>
       <c r="J56" t="n">
-        <v>0.000269804906593583</v>
+        <v>0.000269804906593518</v>
       </c>
       <c r="K56"/>
       <c r="L56" t="n">

</xml_diff>